<commit_message>
Laravel Day - 2
</commit_message>
<xml_diff>
--- a/Laravel-Contens.xlsx
+++ b/Laravel-Contens.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laravel-EG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63E3A6A9-E2BC-43C3-9425-867B6C06DE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2380C5A8-85D7-4553-B656-F14F0D4FF281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-2280" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
     <sheet name="Query-Builder" sheetId="2" r:id="rId2"/>
     <sheet name="Migration" sheetId="3" r:id="rId3"/>
     <sheet name="MIDDLEWARE" sheetId="4" r:id="rId4"/>
+    <sheet name="Validate" sheetId="5" r:id="rId5"/>
+    <sheet name="Image-Libbary" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
   <si>
     <t>Açıklama</t>
   </si>
@@ -626,10 +629,49 @@
 'arakontrol'=&gt;\App\Http\Middleware\FormKontrol::class,</t>
   </si>
   <si>
-    <t>Route::middleware()-&gt;post("/formsonuc",[FormIslemleri::class,'formsonuc'])-&gt;name('formsonuc');</t>
-  </si>
-  <si>
     <t>web.php'de yönlendirmede middelware belirtmemiz lazım postdan önce yazalım ki ilk middelware ' oluşsun</t>
+  </si>
+  <si>
+    <t>Route::middleware('arakontrol')-&gt;post("/formsonuc",[FormIslemleri::class,'formsonuc'])-&gt;name('formsonuc');</t>
+  </si>
+  <si>
+    <t>Migration Oluşturma
+bilgiler -&gt; dosya ismi
+--create=bilgiler  -&gt; tablo ismi
+=&gt; php artisan make:migration bilgiler --create=bilgiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">php artisan migrate </t>
+  </si>
+  <si>
+    <t>migration oluşturduktan sonra bunları vt ye yollamak lazım</t>
+  </si>
+  <si>
+    <t>&gt;php artisan migrat:fresh --seed</t>
+  </si>
+  <si>
+    <t>Validate</t>
+  </si>
+  <si>
+    <t>Gönderilen işlemlerin kontrolünü yapmayı sağlar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compoeser require intervention/image </t>
+  </si>
+  <si>
+    <t>cmd</t>
+  </si>
+  <si>
+    <t>config-&gt;app.php -&gt;providers</t>
+  </si>
+  <si>
+    <t>Intervention\Image\ImageServiceProvide::class,</t>
+  </si>
+  <si>
+    <t>Image' =&gt;Intervention\Image\Facades\Image:class,</t>
+  </si>
+  <si>
+    <t>config-&gt;app.php -&gt;aliases</t>
   </si>
 </sst>
 </file>
@@ -768,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -832,43 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -881,15 +887,64 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1219,10 +1274,10 @@
       <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="23"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="s">
@@ -1461,10 +1516,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D6C69B-9DD3-4D2F-AB49-5ECAD410477F}">
-  <dimension ref="B2:C60"/>
+  <dimension ref="B2:C63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,413 +1558,433 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+    <row r="6" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="31"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="30"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+      <c r="C9" s="39"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="11" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C11" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+    <row r="13" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+    <row r="14" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+    <row r="15" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="30"/>
-    </row>
-    <row r="14" spans="2:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="C16" s="40"/>
+    </row>
+    <row r="17" spans="2:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="30" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="30"/>
-    </row>
-    <row r="16" spans="2:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="C18" s="40"/>
+    </row>
+    <row r="19" spans="2:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="30"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+      <c r="C20" s="40"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="29"/>
-    </row>
-    <row r="19" spans="2:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+      <c r="C21" s="39"/>
+    </row>
+    <row r="22" spans="2:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="29"/>
-    </row>
-    <row r="21" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+      <c r="C23" s="39"/>
+    </row>
+    <row r="24" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="27"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="25"/>
-    </row>
-    <row r="24" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="C26" s="35"/>
+    </row>
+    <row r="27" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C27" s="22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="25"/>
-    </row>
-    <row r="26" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
+      <c r="C28" s="35"/>
+    </row>
+    <row r="29" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
+    <row r="30" spans="2:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C30" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="27"/>
-    </row>
-    <row r="29" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
+      <c r="C31" s="37"/>
+    </row>
+    <row r="32" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C32" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="32"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="21" t="s">
+      <c r="C33" s="42"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B32" s="21" t="s">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C35" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="31" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="32"/>
-    </row>
-    <row r="34" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B34" s="21" t="s">
+      <c r="C36" s="42"/>
+    </row>
+    <row r="37" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C37" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="32"/>
-    </row>
-    <row r="36" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="33" t="s">
+      <c r="C38" s="42"/>
+    </row>
+    <row r="39" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="34"/>
-    </row>
-    <row r="37" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B37" s="21" t="s">
+      <c r="C39" s="44"/>
+    </row>
+    <row r="40" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="31" t="s">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="32"/>
-    </row>
-    <row r="39" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B39" s="21" t="s">
+      <c r="C41" s="42"/>
+    </row>
+    <row r="42" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B42" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C42" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="31" t="s">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="32"/>
-    </row>
-    <row r="41" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="C43" s="42"/>
+    </row>
+    <row r="44" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B44" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="16"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="31" t="s">
+      <c r="C44" s="16"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="32"/>
-    </row>
-    <row r="43" spans="2:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="35" t="s">
+      <c r="C45" s="42"/>
+    </row>
+    <row r="46" spans="2:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="32"/>
-    </row>
-    <row r="44" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B44" s="21" t="s">
+      <c r="C46" s="42"/>
+    </row>
+    <row r="47" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C47" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="31" t="s">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="32"/>
-    </row>
-    <row r="46" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" s="16"/>
-    </row>
-    <row r="47" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B47" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B48" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>119</v>
-      </c>
+      <c r="C48" s="42"/>
     </row>
     <row r="49" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B49" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="16"/>
+    </row>
+    <row r="50" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B50" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B51" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B52" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C52" s="16" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="32"/>
-    </row>
-    <row r="51" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B51" s="21" t="s">
+      <c r="C53" s="42"/>
+    </row>
+    <row r="54" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B54" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C54" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="31" t="s">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="C52" s="32"/>
-    </row>
-    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="21" t="s">
+      <c r="C55" s="42"/>
+    </row>
+    <row r="56" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="16"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>132</v>
-      </c>
+      <c r="C56" s="16"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="21" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C62" s="16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="21"/>
-      <c r="C60" s="16"/>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="21"/>
+      <c r="C63" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B55:C55"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1921,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E59466-D3DB-417D-983B-90E73EE10891}">
   <dimension ref="C3:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,123 +2008,123 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="24" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="26" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="26" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="30" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="8" spans="3:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="39"/>
-      <c r="D14" s="41"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="29"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="39"/>
-      <c r="D15" s="41"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="29"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="39"/>
-      <c r="D16" s="41"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="29"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2058,4 +2133,80 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8AA3C6-FC91-4A7B-ACC6-A4867C7A9AF0}">
+  <dimension ref="B3:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B253D2E-A8CE-4A9E-8CC7-83D8F6E7BCD9}">
+  <dimension ref="B3:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>